<commit_message>
1. Adding SignUp Page class 2. Code refactoring
</commit_message>
<xml_diff>
--- a/Test_Case_Details.xlsx
+++ b/Test_Case_Details.xlsx
@@ -67,9 +67,6 @@
     <t>Upload image/audio/video/doc in media. Ref. http://demo.rtcamp.com/rtmedia/members/admin/media/Note: Replace admin with Your User Name.</t>
   </si>
   <si>
-    <t>Image/audio/video/doc should be uploaded in the selected album and with the selected privacy only successfully</t>
-  </si>
-  <si>
     <t>Upload image/audio/video/doc in media by URL</t>
   </si>
   <si>
@@ -104,6 +101,9 @@
   </si>
   <si>
     <t>TC_009_Upload_Media_By_URL</t>
+  </si>
+  <si>
+    <t>Image/audio/video/doc should be uploaded in the selected album and with the selected privacy only successfully.</t>
   </si>
 </sst>
 </file>
@@ -621,20 +621,20 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="49.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="94.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="72.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="75.85546875" customWidth="1"/>
+    <col min="3" max="3" width="72.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:3" s="6" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>0</v>
@@ -645,7 +645,7 @@
     </row>
     <row r="3" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
@@ -656,7 +656,7 @@
     </row>
     <row r="4" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
@@ -667,7 +667,7 @@
     </row>
     <row r="5" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>6</v>
@@ -678,7 +678,7 @@
     </row>
     <row r="6" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>8</v>
@@ -689,7 +689,7 @@
     </row>
     <row r="7" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>10</v>
@@ -700,7 +700,7 @@
     </row>
     <row r="8" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>12</v>
@@ -711,7 +711,7 @@
     </row>
     <row r="9" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>14</v>
@@ -720,26 +720,26 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:3" s="11" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="10" t="s">
         <v>18</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>

</xml_diff>